<commit_message>
Added environment type (prod or ref)
</commit_message>
<xml_diff>
--- a/data/manual.xlsx
+++ b/data/manual.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patricjansson/dev/kth/gita.sys.kth.se/flottsbro-api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E078974B-B812-B948-B519-CD36257BE1C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6A618C-EF9D-F944-BD94-CC48250D8B5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16420"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="manual" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
-  <si>
-    <t xml:space="preserve"> 1554386577.8160307</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> high</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> https://www.kth.se</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> APPLICATION_STATUS: OK</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="84">
   <si>
     <t>applicationName</t>
   </si>
@@ -64,18 +52,12 @@
     <t>KTH Websites (CMS)</t>
   </si>
   <si>
-    <t>10.0.14</t>
-  </si>
-  <si>
     <t>social</t>
   </si>
   <si>
     <t>master-4.28.0-338</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1558022400.8160307</t>
-  </si>
-  <si>
     <t>Social</t>
   </si>
   <si>
@@ -125,13 +107,178 @@
   </si>
   <si>
     <t>team</t>
+  </si>
+  <si>
+    <t>10.0.14-fbea0b6</t>
+  </si>
+  <si>
+    <t>1554386577.8160307</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>https://www.kth.se</t>
+  </si>
+  <si>
+    <t>APPLICATION_STATUS: OK</t>
+  </si>
+  <si>
+    <t>cortina-edit</t>
+  </si>
+  <si>
+    <t>CMS Redaktörsverktyg</t>
+  </si>
+  <si>
+    <t>CMS Editing tool</t>
+  </si>
+  <si>
+    <t>Redaktörsverktyget för KTH:s webbplatser</t>
+  </si>
+  <si>
+    <t>The editing tool/backend for updating KTH websites</t>
+  </si>
+  <si>
+    <t>https://www-edit.sys.kth.se/polopoly</t>
+  </si>
+  <si>
+    <t>https://www-edit.sys.kth.se/_monitor</t>
+  </si>
+  <si>
+    <t>1558022400.8160307</t>
+  </si>
+  <si>
+    <t>timeedit</t>
+  </si>
+  <si>
+    <t>saas</t>
+  </si>
+  <si>
+    <t>KTH Schema</t>
+  </si>
+  <si>
+    <t>https://cloud.timeedit.net/kth/web/public01/</t>
+  </si>
+  <si>
+    <t>search time tables</t>
+  </si>
+  <si>
+    <t>team-studadm</t>
+  </si>
+  <si>
+    <t>canvas</t>
+  </si>
+  <si>
+    <t>Canvas</t>
+  </si>
+  <si>
+    <t>https://kth.instructure.com/</t>
+  </si>
+  <si>
+    <t>användargodkännande krävs</t>
+  </si>
+  <si>
+    <t>webmail</t>
+  </si>
+  <si>
+    <t>KTH Webmail</t>
+  </si>
+  <si>
+    <t>Webbklient för kth.se-konton</t>
+  </si>
+  <si>
+    <t>Webmail client for kth.se-accounts</t>
+  </si>
+  <si>
+    <t>https://webmail.kth.se</t>
+  </si>
+  <si>
+    <t>ita-ops</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>201502.2-0-gc01a6aa</t>
+  </si>
+  <si>
+    <t>KTH Login Service</t>
+  </si>
+  <si>
+    <t>Inloggning för KTH:s tjänser (SAML, CAS, ADFS...)</t>
+  </si>
+  <si>
+    <t>Single sign on service för kth.se</t>
+  </si>
+  <si>
+    <t>https://login.kth.se</t>
+  </si>
+  <si>
+    <t>https://login.kth.se/_monitor</t>
+  </si>
+  <si>
+    <t>files-web</t>
+  </si>
+  <si>
+    <t>2.5.4</t>
+  </si>
+  <si>
+    <t>KTH Files</t>
+  </si>
+  <si>
+    <t>Hanterar uppladdade filer i KTH Profiles</t>
+  </si>
+  <si>
+    <t>Handles uploaded files in KTH Profiles</t>
+  </si>
+  <si>
+    <t>https://www.kth.se/files</t>
+  </si>
+  <si>
+    <t>https://www.kth.se/files/_monitor</t>
+  </si>
+  <si>
+    <t>files-api</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>Files API</t>
+  </si>
+  <si>
+    <t>https://www.kth.se/api/files</t>
+  </si>
+  <si>
+    <t>https://www.kth.se/api/files/_monitor</t>
+  </si>
+  <si>
+    <t>kth-book-cover</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>KTH Book Cover</t>
+  </si>
+  <si>
+    <t>Skapar exjobbs-omslag</t>
+  </si>
+  <si>
+    <t>Creates covers for master thesis reports</t>
+  </si>
+  <si>
+    <t>https://intra.kth.se/kth-cover</t>
+  </si>
+  <si>
+    <t>https://intra.kth.se/kth-cover/_monitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,6 +431,38 @@
       <sz val="12"/>
       <color rgb="FFCE9178"/>
       <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -629,18 +808,16 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -996,11 +1173,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1017,134 +1194,454 @@
     <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="F2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="Q2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="K7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>34</v>
+      <c r="R8" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="H9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="K9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="7">
+        <v>8</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="K3" r:id="rId3"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{46970FFA-5C5E-4E40-AC96-CB16D3BC1FE3}"/>
+    <hyperlink ref="P5" r:id="rId2" xr:uid="{1FF11C8C-7BA6-E04D-8AD5-35F87E806008}"/>
+    <hyperlink ref="O6" r:id="rId3" xr:uid="{55B91F0D-D9D6-7F45-AB06-EF1F71C2A2EF}"/>
+    <hyperlink ref="P6" r:id="rId4" xr:uid="{27162707-1D88-9F40-8850-183D4442D9F1}"/>
+    <hyperlink ref="O7" r:id="rId5" display="https://webmail.kth.se/" xr:uid="{CE9CBA6C-A008-B94A-9D46-DBC568203EAC}"/>
+    <hyperlink ref="O8" r:id="rId6" display="https://login.kth.se/" xr:uid="{F604EE2F-A4E0-DD4A-BE78-F4FA0933FCF4}"/>
+    <hyperlink ref="P8" r:id="rId7" xr:uid="{6DA23716-08E6-CD4D-ABDE-DF4415524565}"/>
+    <hyperlink ref="O9" r:id="rId8" xr:uid="{359B8E8E-52CC-944A-97EF-973812848474}"/>
+    <hyperlink ref="P9" r:id="rId9" xr:uid="{3576CE32-042C-344A-B23A-CB24933F1028}"/>
+    <hyperlink ref="O10" r:id="rId10" xr:uid="{CF1A222D-3B79-5142-A95D-6B9852BEF514}"/>
+    <hyperlink ref="P10" r:id="rId11" xr:uid="{F8241432-46FA-A647-97C1-ACE93401A20D}"/>
+    <hyperlink ref="O11" r:id="rId12" xr:uid="{B7FD0806-45B2-3449-BBB4-481A7FEAC850}"/>
+    <hyperlink ref="P11" r:id="rId13" xr:uid="{58F89650-921E-884F-8DE3-1376D5E17B03}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>